<commit_message>
Fixed column name in BOM.
</commit_message>
<xml_diff>
--- a/cam/USB2Serial_CH340G_v1.0_2020-10-22-BOM.xlsx
+++ b/cam/USB2Serial_CH340G_v1.0_2020-10-22-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\USB2Serial\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194D04A0-DAD8-44B0-9A22-FF8B609F4E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474159A-350A-43C6-BBB7-82AB7DFC3F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="20" windowWidth="20880" windowHeight="20940" xr2:uid="{31E49BBC-3A94-4FF3-A947-B65A54B65835}"/>
+    <workbookView xWindow="8420" yWindow="180" windowWidth="22180" windowHeight="20940" xr2:uid="{31E49BBC-3A94-4FF3-A947-B65A54B65835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>JCSC Part #</t>
-  </si>
-  <si>
     <t>0402</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>C1017</t>
+  </si>
+  <si>
+    <t>LCSC Part #</t>
   </si>
 </sst>
 </file>
@@ -269,7 +269,7 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -278,7 +278,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -334,11 +334,11 @@
   <autoFilter ref="A1:F13" xr:uid="{BAB39257-4E9E-40F8-9461-DACDAEF43607}"/>
   <tableColumns count="6">
     <tableColumn id="20" xr3:uid="{717A90BC-AFF8-427A-B1D8-59849719859C}" uniqueName="20" name="Qty" queryTableFieldId="1"/>
-    <tableColumn id="22" xr3:uid="{4F70E942-F885-48B7-A1A3-E716663C5806}" uniqueName="22" name="Designator" queryTableFieldId="21" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{FCAC85D0-BBE6-4A0A-BCA2-14613D5AEB21}" uniqueName="23" name="Footprint" queryTableFieldId="22" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{795927D8-D924-41E3-9752-8929A124819C}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{A73A3260-BD4C-44FD-9186-57FD632844EF}" uniqueName="25" name="JCSC Part #" queryTableFieldId="23" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{645F92FB-5D06-411C-BB9F-FCAE6B822555}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{4F70E942-F885-48B7-A1A3-E716663C5806}" uniqueName="22" name="Designator" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{FCAC85D0-BBE6-4A0A-BCA2-14613D5AEB21}" uniqueName="23" name="Footprint" queryTableFieldId="22" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{795927D8-D924-41E3-9752-8929A124819C}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{A73A3260-BD4C-44FD-9186-57FD632844EF}" uniqueName="25" name="LCSC Part #" queryTableFieldId="23" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{645F92FB-5D06-411C-BB9F-FCAE6B822555}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA13B97C-AC77-41DE-8A85-C8BB9D639B68}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -686,16 +686,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -706,16 +706,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -726,16 +726,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -746,13 +746,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -766,16 +766,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -786,16 +786,16 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -806,16 +806,16 @@
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -826,13 +826,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
@@ -846,16 +846,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -866,13 +866,13 @@
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
@@ -886,16 +886,16 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -906,13 +906,13 @@
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>

</xml_diff>